<commit_message>
fixed tile column to have position number instead of name
</commit_message>
<xml_diff>
--- a/code/ExcelData/PropertyTycoonCardDataRefactored.xlsx
+++ b/code/ExcelData/PropertyTycoonCardDataRefactored.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\Files\Project\Monopoly-Game\code\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4AECD30-F9A6-481D-9699-0F95417EB04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF1AA4-9119-40FB-8715-7072FD9DB79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="3405" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="5895" yWindow="1680" windowWidth="14220" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>Potluck card</t>
   </si>
@@ -97,19 +97,10 @@
     <t>pass go</t>
   </si>
   <si>
-    <t>old creek</t>
-  </si>
-  <si>
     <t>"You are up the creek with no paddle - go back to the Old Creek"</t>
   </si>
   <si>
-    <t>go</t>
-  </si>
-  <si>
     <t>"Advance to go"</t>
-  </si>
-  <si>
-    <t>jail</t>
   </si>
   <si>
     <t>"Go to jail. Do not pass GO, do not collect £200"</t>
@@ -181,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,12 +533,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -557,14 +550,13 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -578,7 +570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -592,7 +584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -606,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -620,7 +612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -634,7 +626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -648,7 +640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -662,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -676,7 +668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -690,7 +682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -704,7 +696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -718,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -732,7 +724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -746,7 +738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -760,7 +752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -774,64 +766,60 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
+      <c r="B19">
+        <v>2</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" t="b">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
+      <c r="B21">
+        <v>11</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
@@ -845,7 +833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -856,10 +844,10 @@
         <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -870,10 +858,10 @@
         <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -884,10 +872,10 @@
         <v>150</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -898,24 +886,24 @@
         <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -926,11 +914,10 @@
         <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
@@ -938,16 +925,16 @@
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -961,10 +948,10 @@
         <v>115</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -978,13 +965,12 @@
         <v>100</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>23</v>
@@ -993,10 +979,10 @@
         <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="b">
         <v>1</v>
       </c>
@@ -1007,10 +993,10 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="b">
         <v>1</v>
       </c>
@@ -1021,10 +1007,10 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="b">
         <v>1</v>
       </c>
@@ -1035,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="b">
         <v>1</v>
       </c>
@@ -1049,10 +1035,10 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="b">
         <v>0</v>
       </c>
@@ -1063,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="b">
         <v>1</v>
       </c>
@@ -1077,10 +1063,10 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="b">
         <v>1</v>
       </c>
@@ -1091,25 +1077,14 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.25"/>
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
fixed jail card data in excel
</commit_message>
<xml_diff>
--- a/code/ExcelData/PropertyTycoonCardDataRefactored.xlsx
+++ b/code/ExcelData/PropertyTycoonCardDataRefactored.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Desktop\Files\Project\Monopoly-Game\code\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BF1AA4-9119-40FB-8715-7072FD9DB79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE4906C-8F04-48D9-80BF-B96E3DE1FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="1680" windowWidth="14220" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>Potluck card</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>"Advance to Skywalker Drive. If you pass GO collect £200"</t>
+  </si>
+  <si>
+    <t>Get out of jail free</t>
   </si>
 </sst>
 </file>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +816,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
@@ -1083,6 +1091,11 @@
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>